<commit_message>
result output was corrected
</commit_message>
<xml_diff>
--- a/output_logic_ctrlunit_datafetch.xlsx
+++ b/output_logic_ctrlunit_datafetch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="10500" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="10500" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t xml:space="preserve"> q1</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>loaddp0</t>
-  </si>
-  <si>
-    <t>loadbp</t>
   </si>
   <si>
     <t>selmuxdp1</t>
@@ -521,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,20 +529,19 @@
     <col min="1" max="8" width="6.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="1" customWidth="1"/>
     <col min="10" max="11" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -553,17 +549,16 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="J1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="P1" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -571,22 +566,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>3</v>
@@ -600,12 +595,9 @@
       <c r="M2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="11"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -643,15 +635,12 @@
       <c r="M3" s="4">
         <v>0</v>
       </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N3" s="5"/>
+      <c r="O3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -688,285 +677,264 @@
       <c r="M4" s="1">
         <v>0</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="9" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="9" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="9" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1</v>
-      </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="9" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="9" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1001,20 +969,17 @@
         <v>1</v>
       </c>
       <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1046,17 +1011,14 @@
         <v>1</v>
       </c>
       <c r="L13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1088,17 +1050,14 @@
         <v>1</v>
       </c>
       <c r="L14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1133,14 +1092,11 @@
         <v>1</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1172,17 +1128,14 @@
         <v>1</v>
       </c>
       <c r="L16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
       </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1214,17 +1167,14 @@
         <v>1</v>
       </c>
       <c r="L17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1259,14 +1209,11 @@
         <v>1</v>
       </c>
       <c r="M18" s="1">
-        <v>1</v>
-      </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="P18"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1301,14 +1248,11 @@
         <v>1</v>
       </c>
       <c r="M19" s="1">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1">
-        <v>0</v>
-      </c>
-      <c r="P19"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1343,17 +1287,14 @@
         <v>1</v>
       </c>
       <c r="M20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="P20"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1385,17 +1326,14 @@
         <v>0</v>
       </c>
       <c r="L22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1427,17 +1365,14 @@
         <v>0</v>
       </c>
       <c r="L23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="1">
         <v>0</v>
       </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1469,17 +1404,14 @@
         <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>1</v>
-      </c>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1514,14 +1446,11 @@
         <v>1</v>
       </c>
       <c r="M25" s="1">
-        <v>1</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1556,14 +1485,11 @@
         <v>1</v>
       </c>
       <c r="M26" s="1">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1595,17 +1521,14 @@
         <v>0</v>
       </c>
       <c r="L27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="1">
         <v>0</v>
       </c>
-      <c r="N27" s="1">
-        <v>0</v>
-      </c>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1640,14 +1563,11 @@
         <v>1</v>
       </c>
       <c r="M28" s="1">
-        <v>1</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1682,17 +1602,14 @@
         <v>1</v>
       </c>
       <c r="M29" s="1">
-        <v>1</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1727,14 +1644,11 @@
         <v>1</v>
       </c>
       <c r="M31" s="1">
-        <v>1</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0</v>
-      </c>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1769,14 +1683,11 @@
         <v>1</v>
       </c>
       <c r="M32" s="1">
-        <v>1</v>
-      </c>
-      <c r="N32" s="1">
-        <v>0</v>
-      </c>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1811,14 +1722,11 @@
         <v>1</v>
       </c>
       <c r="M33" s="1">
-        <v>1</v>
-      </c>
-      <c r="N33" s="1">
-        <v>0</v>
-      </c>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1853,14 +1761,11 @@
         <v>1</v>
       </c>
       <c r="M34" s="1">
-        <v>1</v>
-      </c>
-      <c r="N34" s="1">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1895,14 +1800,11 @@
         <v>1</v>
       </c>
       <c r="M35" s="1">
-        <v>1</v>
-      </c>
-      <c r="N35" s="1">
-        <v>0</v>
-      </c>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1937,14 +1839,11 @@
         <v>1</v>
       </c>
       <c r="M36" s="1">
-        <v>1</v>
-      </c>
-      <c r="N36" s="1">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1979,14 +1878,11 @@
         <v>1</v>
       </c>
       <c r="M37" s="1">
-        <v>1</v>
-      </c>
-      <c r="N37" s="1">
-        <v>0</v>
-      </c>
-      <c r="O37" s="1"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -2021,30 +1917,27 @@
         <v>1</v>
       </c>
       <c r="M38" s="1">
-        <v>1</v>
-      </c>
-      <c r="N38" s="1">
-        <v>0</v>
-      </c>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O42" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>